<commit_message>
update module upload new student
</commit_message>
<xml_diff>
--- a/assets/files/Student_From_Data.xlsx
+++ b/assets/files/Student_From_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/fieldwork_nuol/assets/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE9B0E2-F6FA-F949-8A2B-1F847085659D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46F2057-D07C-7C43-AF38-0C00DA893455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{F46E6FF6-3060-2745-AE4A-2972A309CDBC}"/>
   </bookViews>
@@ -168,33 +168,39 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -514,12 +520,12 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="10.83203125" style="4"/>
     <col min="2" max="4" width="10.83203125" style="1"/>
     <col min="5" max="6" width="21.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.83203125" style="1" customWidth="1"/>
@@ -568,24 +574,25 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="Gu0DMrwQMqqneapbvAyrK/kjILun4zQeFkx5ValHwizCjm5m0R8HIvG/2wnkmQGFRik6xy8X5ORHcWIdc1YEig==" saltValue="9I9fPR1om43eEfdMUJXIMA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>

</xml_diff>